<commit_message>
envio de email al empleado
</commit_message>
<xml_diff>
--- a/public/archives/PLANTILLA-DE-REGISTRO-PARA-ASEGURADOS.xlsx
+++ b/public/archives/PLANTILLA-DE-REGISTRO-PARA-ASEGURADOS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan_\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan_\Desktop\Agua e' Panela\Red Bucal\red-bucal\public\archives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3F66F3-441A-49A6-BDDA-4672ED81A498}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81F71B8-B2AD-4901-83F6-22BDE6B5CB1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>INDIVIDUALES REFERIDOS</t>
   </si>
@@ -130,6 +130,12 @@
   <si>
     <t>F. NACIMIENTO*
 (El formato de la fecha debe ser DD/MM/AA)</t>
+  </si>
+  <si>
+    <t>TYPO:</t>
+  </si>
+  <si>
+    <t>Asegurados</t>
   </si>
 </sst>
 </file>
@@ -254,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -286,6 +292,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -295,7 +304,8 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -320,15 +330,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>377135</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>157620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1764665</xdr:colOff>
+      <xdr:colOff>1976700</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>151130</xdr:rowOff>
+      <xdr:rowOff>27041</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -349,8 +359,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="165100" y="292100"/>
-          <a:ext cx="1599565" cy="430530"/>
+          <a:off x="377135" y="157620"/>
+          <a:ext cx="1599565" cy="426012"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -368,7 +378,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -666,11 +676,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:L13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="40.109375" style="1" customWidth="1"/>
@@ -689,202 +699,206 @@
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="13"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+    </row>
+    <row r="5" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
     </row>
     <row r="6" spans="1:14" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B7" s="14"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
+      <c r="A8" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
     </row>
     <row r="9" spans="1:14" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
+      <c r="A9" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
     </row>
     <row r="10" spans="1:14" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
     </row>
     <row r="11" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="17">
         <v>0.7</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
     </row>
     <row r="12" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
     </row>
     <row r="14" spans="1:14" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
@@ -899,364 +913,364 @@
       <c r="D14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
     </row>
     <row r="15" spans="1:14" s="8" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
     </row>
     <row r="16" spans="1:14" s="8" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
     </row>
     <row r="17" spans="1:12" s="8" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
     </row>
     <row r="18" spans="1:12" s="8" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
     </row>
     <row r="19" spans="1:12" s="8" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
     </row>
     <row r="20" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
     </row>
     <row r="21" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
     </row>
     <row r="22" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
     </row>
     <row r="23" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
     </row>
     <row r="24" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
     </row>
     <row r="25" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
     </row>
     <row r="26" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
     </row>
     <row r="27" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
     </row>
     <row r="28" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
     </row>
     <row r="29" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
     </row>
     <row r="30" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
     </row>
     <row r="31" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
     </row>
     <row r="32" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
     </row>
     <row r="33" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
     </row>
     <row r="34" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
     </row>
     <row r="35" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
     </row>
     <row r="36" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="17"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
     </row>
     <row r="37" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
     </row>
     <row r="38" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="17"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
     </row>
     <row r="39" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="17"/>
-      <c r="K39" s="17"/>
-      <c r="L39" s="17"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>